<commit_message>
created char generator class that will generate charts for pdfs and xlsx
</commit_message>
<xml_diff>
--- a/xlsxdoc.xlsx
+++ b/xlsxdoc.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Kacper</t>
   </si>
@@ -22,7 +22,7 @@
   </si>
   <si>
     <t>Report Generated on:
-09/01/2024 11:51:17</t>
+09/01/2024 12:07:12</t>
   </si>
   <si>
     <t>Balance:
@@ -228,9 +228,110 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" rtlCol="false"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Expenses by Category</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="false"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Expenses</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Transactions!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Category</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Transactions!$B$9</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="false"/>
+    </c:legend>
+    <c:plotVisOnly val="true"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Diagramm0"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="10772775" cy="3429000"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -292,141 +393,78 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>18</v>
+      <c r="B10" t="n" s="0">
+        <v>150.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>0.32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>4000.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="B13" t="n" s="0">
+        <v>3000.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s" s="0">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="B14" t="n" s="0">
+        <v>1800.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="E15" t="s" s="0">
-        <v>36</v>
+        <v>13</v>
+      </c>
+      <c r="B15" t="n" s="0">
+        <v>5005.01</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B16" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D16" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="E16" t="s" s="0">
-        <v>40</v>
+      <c r="B17" t="n" s="0">
+        <v>200.0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>